<commit_message>
vlookup, sum, sumif, sumifs, separate data and concate data
</commit_message>
<xml_diff>
--- a/Day_1_Rumus Excel/Project-Management-Sample-Data.xlsx
+++ b/Day_1_Rumus Excel/Project-Management-Sample-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Music\Excel Data for Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shopi Upgrade Skill\30_days_excel-fuundamental\Day_1_Rumus Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FD8F0A-8B7C-4098-8505-230CA176550F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB35B5D-07D6-426C-8FF9-E9F761E47599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE120CA2-B4E2-4FC9-9B81-FB00098FDFE6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{CE120CA2-B4E2-4FC9-9B81-FB00098FDFE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Management Data" sheetId="2" r:id="rId1"/>
@@ -23,12 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="114">
   <si>
     <t>Excel Sample Data</t>
   </si>
@@ -372,13 +367,19 @@
   </si>
   <si>
     <t>Tom</t>
+  </si>
+  <si>
+    <t>IFERROR</t>
+  </si>
+  <si>
+    <t>VLOOKUP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -840,26 +841,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC7BEC1-BD91-4F4F-8985-8014BC582418}">
-  <dimension ref="B2:H52"/>
+  <dimension ref="B2:J52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="18" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="25" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="13.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="17" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="2"/>
+    <col min="9" max="16384" width="9.125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:10" ht="18" customHeight="1" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -870,7 +870,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="4" spans="2:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="18" customHeight="1" thickBot="1">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -881,7 +881,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="6" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="18" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
@@ -903,8 +903,14 @@
       <c r="H6" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="18" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
@@ -927,7 +933,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="18" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
@@ -950,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="18" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
@@ -973,7 +979,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="18" customHeight="1">
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
@@ -996,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="18" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
@@ -1019,7 +1025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="18" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
@@ -1042,7 +1048,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="18" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="18" customHeight="1">
       <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1088,7 +1094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="18" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
@@ -1111,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="18" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
@@ -1134,7 +1140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="18" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>32</v>
       </c>
@@ -1157,7 +1163,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="18" customHeight="1">
       <c r="B18" s="5" t="s">
         <v>32</v>
       </c>
@@ -1180,7 +1186,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" ht="18" customHeight="1">
       <c r="B19" s="5" t="s">
         <v>32</v>
       </c>
@@ -1203,7 +1209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="18" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>38</v>
       </c>
@@ -1226,7 +1232,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="18" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>38</v>
       </c>
@@ -1249,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="18" customHeight="1">
       <c r="B22" s="5" t="s">
         <v>38</v>
       </c>
@@ -1272,7 +1278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="18" customHeight="1">
       <c r="B23" s="5" t="s">
         <v>45</v>
       </c>
@@ -1295,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="18" customHeight="1">
       <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
@@ -1318,7 +1324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="18" customHeight="1">
       <c r="B25" s="5" t="s">
         <v>45</v>
       </c>
@@ -1341,7 +1347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" ht="18" customHeight="1">
       <c r="B26" s="5" t="s">
         <v>52</v>
       </c>
@@ -1364,7 +1370,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" ht="18" customHeight="1">
       <c r="B27" s="5" t="s">
         <v>52</v>
       </c>
@@ -1387,7 +1393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" ht="18" customHeight="1">
       <c r="B28" s="5" t="s">
         <v>52</v>
       </c>
@@ -1410,7 +1416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" ht="18" customHeight="1">
       <c r="B29" s="5" t="s">
         <v>59</v>
       </c>
@@ -1433,7 +1439,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" ht="18" customHeight="1">
       <c r="B30" s="5" t="s">
         <v>59</v>
       </c>
@@ -1456,7 +1462,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" ht="18" customHeight="1">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
@@ -1479,7 +1485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" ht="18" customHeight="1">
       <c r="B32" s="5" t="s">
         <v>66</v>
       </c>
@@ -1502,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" ht="18" customHeight="1">
       <c r="B33" s="5" t="s">
         <v>66</v>
       </c>
@@ -1525,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" ht="18" customHeight="1">
       <c r="B34" s="5" t="s">
         <v>66</v>
       </c>
@@ -1548,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" ht="18" customHeight="1">
       <c r="B35" s="5" t="s">
         <v>73</v>
       </c>
@@ -1571,7 +1577,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" ht="18" customHeight="1">
       <c r="B36" s="5" t="s">
         <v>73</v>
       </c>
@@ -1594,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" ht="18" customHeight="1">
       <c r="B37" s="5" t="s">
         <v>73</v>
       </c>
@@ -1617,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" ht="18" customHeight="1">
       <c r="B38" s="5" t="s">
         <v>80</v>
       </c>
@@ -1640,7 +1646,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" ht="18" customHeight="1">
       <c r="B39" s="5" t="s">
         <v>80</v>
       </c>
@@ -1663,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" ht="18" customHeight="1">
       <c r="B40" s="5" t="s">
         <v>80</v>
       </c>
@@ -1686,7 +1692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" ht="18" customHeight="1">
       <c r="B41" s="5" t="s">
         <v>86</v>
       </c>
@@ -1709,7 +1715,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" ht="18" customHeight="1">
       <c r="B42" s="5" t="s">
         <v>86</v>
       </c>
@@ -1732,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" ht="18" customHeight="1">
       <c r="B43" s="5" t="s">
         <v>86</v>
       </c>
@@ -1755,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:8" ht="18" customHeight="1">
       <c r="B44" s="5" t="s">
         <v>93</v>
       </c>
@@ -1778,7 +1784,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" ht="18" customHeight="1">
       <c r="B45" s="5" t="s">
         <v>93</v>
       </c>
@@ -1801,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:8" ht="18" customHeight="1">
       <c r="B46" s="5" t="s">
         <v>93</v>
       </c>
@@ -1824,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:8" ht="18" customHeight="1">
       <c r="B47" s="5" t="s">
         <v>100</v>
       </c>
@@ -1847,7 +1853,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:8" ht="18" customHeight="1">
       <c r="B48" s="5" t="s">
         <v>100</v>
       </c>
@@ -1870,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:8" ht="18" customHeight="1">
       <c r="B49" s="5" t="s">
         <v>100</v>
       </c>
@@ -1893,7 +1899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:8" ht="18" customHeight="1">
       <c r="B50" s="5" t="s">
         <v>107</v>
       </c>
@@ -1916,7 +1922,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:8" ht="18" customHeight="1">
       <c r="B51" s="5" t="s">
         <v>107</v>
       </c>
@@ -1939,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:8" ht="18" customHeight="1">
       <c r="B52" s="5" t="s">
         <v>107</v>
       </c>
@@ -1964,5 +1970,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>